<commit_message>
changing the logic to make the changes reflect on the original file
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/ColorFormat/output1.xlsx
+++ b/src/test/resources/test_files/ColorFormat/output1.xlsx
@@ -136,12 +136,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="12"/>
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -482,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
@@ -494,7 +494,7 @@
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" s="0">
+      <c r="B1" s="1">
         <v>100</v>
       </c>
       <c r="C1" t="s" s="0">
@@ -511,7 +511,7 @@
       <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2" s="1">
         <v>200</v>
       </c>
       <c r="C2" t="s" s="0">
@@ -528,7 +528,7 @@
       <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3" s="1">
         <v>300</v>
       </c>
       <c r="C3" t="s" s="0">
@@ -545,7 +545,7 @@
       <c r="A4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4" s="1">
         <v>200</v>
       </c>
       <c r="C4" t="s" s="0">
@@ -559,28 +559,27 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s" s="1">
+      <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>500</v>
       </c>
-      <c r="C5" t="s" s="1">
+      <c r="C5" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="0">
         <v>5.5</v>
       </c>
-      <c r="E5" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1"/>
+      <c r="E5" t="s" s="0">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6" s="1">
         <v>100</v>
       </c>
       <c r="C6" t="s" s="0">
@@ -597,7 +596,7 @@
       <c r="A7" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7" s="1">
         <v>200</v>
       </c>
       <c r="C7" t="s" s="0">
@@ -614,7 +613,7 @@
       <c r="A8" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8" s="1">
         <v>300</v>
       </c>
       <c r="C8" t="s" s="0">
@@ -631,7 +630,7 @@
       <c r="A9" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9" s="1">
         <v>200</v>
       </c>
       <c r="C9" t="s" s="0">
@@ -648,7 +647,7 @@
       <c r="A10" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10" s="1">
         <v>500</v>
       </c>
       <c r="C10" t="s" s="0">
@@ -665,7 +664,7 @@
       <c r="A11" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11" s="1">
         <v>100</v>
       </c>
       <c r="C11" t="s" s="0">
@@ -682,7 +681,7 @@
       <c r="A12" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B12" s="0">
+      <c r="B12" s="1">
         <v>200</v>
       </c>
       <c r="C12" t="s" s="0">
@@ -699,7 +698,7 @@
       <c r="A13" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13" s="1">
         <v>300</v>
       </c>
       <c r="C13" t="s" s="0">
@@ -716,7 +715,7 @@
       <c r="A14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14" s="1">
         <v>200</v>
       </c>
       <c r="C14" t="s" s="0">
@@ -733,7 +732,7 @@
       <c r="A15" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15" s="1">
         <v>500</v>
       </c>
       <c r="C15" t="s" s="0">
@@ -750,7 +749,7 @@
       <c r="A16" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16" s="1">
         <v>328.57142857142901</v>
       </c>
       <c r="C16" t="s" s="0">
@@ -767,7 +766,7 @@
       <c r="A17" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17" s="1">
         <v>337.142857142857</v>
       </c>
       <c r="C17" t="s" s="0">
@@ -784,7 +783,7 @@
       <c r="A18" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18" s="1">
         <v>345.71428571428601</v>
       </c>
       <c r="C18" t="s" s="0">
@@ -801,7 +800,7 @@
       <c r="A19" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19" s="1">
         <v>354.28571428571399</v>
       </c>
       <c r="C19" t="s" s="0">
@@ -818,7 +817,7 @@
       <c r="A20" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20" s="1">
         <v>362.857142857143</v>
       </c>
       <c r="C20" t="s" s="0">
@@ -835,7 +834,7 @@
       <c r="A21" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21" s="1">
         <v>371.42857142857099</v>
       </c>
       <c r="C21" t="s" s="0">
@@ -852,7 +851,7 @@
       <c r="A22" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22" s="1">
         <v>380</v>
       </c>
       <c r="C22" t="s" s="0">
@@ -869,7 +868,7 @@
       <c r="A23" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23" s="1">
         <v>388.57142857142901</v>
       </c>
       <c r="C23" t="s" s="0">
@@ -886,7 +885,7 @@
       <c r="A24" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B24" s="0">
+      <c r="B24" s="1">
         <v>397.142857142857</v>
       </c>
       <c r="C24" t="s" s="0">
@@ -903,7 +902,7 @@
       <c r="A25" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B25" s="0">
+      <c r="B25" s="1">
         <v>405.71428571428601</v>
       </c>
       <c r="C25" t="s" s="0">
@@ -920,7 +919,7 @@
       <c r="A26" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B26" s="0">
+      <c r="B26" s="1">
         <v>414.28571428571399</v>
       </c>
       <c r="C26" t="s" s="0">
@@ -937,7 +936,7 @@
       <c r="A27" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B27" s="0">
+      <c r="B27" s="1">
         <v>422.857142857143</v>
       </c>
       <c r="C27" t="s" s="0">
@@ -954,7 +953,7 @@
       <c r="A28" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B28" s="0">
+      <c r="B28" s="1">
         <v>431.42857142857099</v>
       </c>
       <c r="C28" t="s" s="0">
@@ -971,7 +970,7 @@
       <c r="A29" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B29" s="0">
+      <c r="B29" s="1">
         <v>440</v>
       </c>
       <c r="C29" t="s" s="0">
@@ -988,7 +987,7 @@
       <c r="A30" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B30" s="0">
+      <c r="B30" s="1">
         <v>448.57142857142799</v>
       </c>
       <c r="C30" t="s" s="0">
@@ -1005,7 +1004,7 @@
       <c r="A31" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B31" s="0">
+      <c r="B31" s="1">
         <v>457.142857142857</v>
       </c>
       <c r="C31" t="s" s="0">
@@ -1022,7 +1021,7 @@
       <c r="A32" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B32" s="0">
+      <c r="B32" s="1">
         <v>465.71428571428601</v>
       </c>
       <c r="C32" t="s" s="0">
@@ -1039,7 +1038,7 @@
       <c r="A33" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B33" s="0">
+      <c r="B33" s="1">
         <v>474.28571428571399</v>
       </c>
       <c r="C33" t="s" s="0">
@@ -1056,7 +1055,7 @@
       <c r="A34" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B34" s="0">
+      <c r="B34" s="1">
         <v>482.857142857143</v>
       </c>
       <c r="C34" t="s" s="0">

</xml_diff>